<commit_message>
moved save before cham_up
saving results before calling cham_up in ode_updater means that saved results represent the condition before any instantaneous changes (such as particle injection) at the saved time.
</commit_message>
<xml_diff>
--- a/PyCHAM/input/ind_AQ_ex/const_infl.xlsx
+++ b/PyCHAM/input/ind_AQ_ex/const_infl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Simon_OMeara/Desktop/PyCHAM/PyCHAM/input/ind_AQ_ex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFC2836-9F11-0B46-BDF2-EC049CD08B00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F91BB1D-1958-E64F-8E6E-7353CE343825}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="460" windowWidth="17980" windowHeight="11840" xr2:uid="{A12B527E-AFAD-6348-8F8E-CC39D59E777A}"/>
+    <workbookView xWindow="10720" yWindow="460" windowWidth="14880" windowHeight="8800" xr2:uid="{A12B527E-AFAD-6348-8F8E-CC39D59E777A}"/>
   </bookViews>
   <sheets>
     <sheet name="const_infl" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="175">
   <si>
     <t>CO</t>
   </si>
@@ -1010,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9915D14-D182-E247-B384-ACBF32C9043F}">
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:N76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1023,9 +1023,15 @@
     <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1050,34 +1056,70 @@
       <c r="H1" s="4">
         <v>72900</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="4">
+        <v>111600</v>
+      </c>
+      <c r="J1" s="16">
+        <v>112200</v>
+      </c>
+      <c r="K1" s="4">
+        <v>151200</v>
+      </c>
+      <c r="L1" s="16">
+        <v>152400</v>
+      </c>
+      <c r="M1" s="16">
+        <v>158400</v>
+      </c>
+      <c r="N1" s="16">
+        <v>159300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>4.8000000000000001E-5</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C2" s="4">
-        <v>7.2999999999999999E-5</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="D2" s="4">
-        <v>7.2999999999999999E-5</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="E2" s="4">
-        <v>7.2999999999999999E-5</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="F2" s="4">
-        <v>4.8000000000000001E-5</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G2" s="4">
-        <v>4.8000000000000001E-5</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="H2" s="4">
-        <v>4.8000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="J2" s="4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="K2" s="4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L2" s="4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="M2" s="4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="N2" s="4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1091,7 +1133,7 @@
         <v>0.70299999999999996</v>
       </c>
       <c r="E3" s="7">
-        <v>0.70299999999999996</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="F3" s="7">
         <v>0.22800000000000001</v>
@@ -1102,8 +1144,26 @@
       <c r="H3" s="7">
         <v>0.22800000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I3" s="7">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="K3" s="7">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0.22800000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1177,7 @@
         <v>2.0320000000000001E-4</v>
       </c>
       <c r="E4" s="4">
-        <v>2.0320000000000001E-4</v>
+        <v>1.032E-4</v>
       </c>
       <c r="F4" s="4">
         <v>1.032E-4</v>
@@ -1128,8 +1188,26 @@
       <c r="H4" s="4">
         <v>1.032E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="4">
+        <v>2.0320000000000001E-4</v>
+      </c>
+      <c r="J4" s="4">
+        <v>2.0320000000000001E-4</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1.032E-4</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1.032E-4</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1.032E-4</v>
+      </c>
+      <c r="N4" s="4">
+        <v>1.032E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1154,8 +1232,26 @@
       <c r="H5" s="4">
         <v>7.0200000000000004E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="4">
+        <v>1.4E-3</v>
+      </c>
+      <c r="J5" s="4">
+        <v>1.4E-3</v>
+      </c>
+      <c r="K5" s="4">
+        <v>7.0200000000000004E-4</v>
+      </c>
+      <c r="L5" s="4">
+        <v>7.0200000000000004E-4</v>
+      </c>
+      <c r="M5" s="4">
+        <v>7.0200000000000004E-4</v>
+      </c>
+      <c r="N5" s="4">
+        <v>7.0200000000000004E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1168,8 +1264,8 @@
       <c r="D6" s="4">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="E6" s="4">
-        <v>2.7000000000000001E-3</v>
+      <c r="E6" s="8">
+        <v>5.1599999999999997E-4</v>
       </c>
       <c r="F6" s="8">
         <v>5.1599999999999997E-4</v>
@@ -1180,8 +1276,26 @@
       <c r="H6" s="8">
         <v>5.1599999999999997E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="4">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="K6" s="8">
+        <v>5.1599999999999997E-4</v>
+      </c>
+      <c r="L6" s="8">
+        <v>5.1599999999999997E-4</v>
+      </c>
+      <c r="M6" s="8">
+        <v>5.1599999999999997E-4</v>
+      </c>
+      <c r="N6" s="8">
+        <v>5.1599999999999997E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1195,7 +1309,7 @@
         <v>2.9839999999999998E-2</v>
       </c>
       <c r="E7" s="4">
-        <v>2.9839999999999998E-2</v>
+        <v>1.1039999999999999E-3</v>
       </c>
       <c r="F7" s="4">
         <v>1.1039999999999999E-3</v>
@@ -1206,8 +1320,26 @@
       <c r="H7" s="4">
         <v>1.1039999999999999E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="4">
+        <v>2.9839999999999998E-2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>2.9839999999999998E-2</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1.1039999999999999E-3</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1.1039999999999999E-3</v>
+      </c>
+      <c r="M7" s="4">
+        <v>1.1039999999999999E-3</v>
+      </c>
+      <c r="N7" s="4">
+        <v>1.1039999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>61</v>
       </c>
@@ -1232,8 +1364,26 @@
       <c r="H8" s="4">
         <v>1.1999999999999999E-6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>0</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1.1999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>62</v>
       </c>
@@ -1247,19 +1397,37 @@
         <v>7.3999999999999999E-4</v>
       </c>
       <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
         <v>7.3999999999999999E-4</v>
       </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J9" s="4">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>63</v>
       </c>
@@ -1273,7 +1441,7 @@
         <v>1.0319999999999999E-3</v>
       </c>
       <c r="E10" s="4">
-        <v>1.0319999999999999E-3</v>
+        <v>8.52E-4</v>
       </c>
       <c r="F10" s="4">
         <v>8.52E-4</v>
@@ -1284,8 +1452,26 @@
       <c r="H10" s="4">
         <v>8.52E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="4">
+        <v>1.0319999999999999E-3</v>
+      </c>
+      <c r="J10" s="4">
+        <v>1.0319999999999999E-3</v>
+      </c>
+      <c r="K10" s="4">
+        <v>8.52E-4</v>
+      </c>
+      <c r="L10" s="4">
+        <v>8.52E-4</v>
+      </c>
+      <c r="M10" s="4">
+        <v>8.52E-4</v>
+      </c>
+      <c r="N10" s="4">
+        <v>8.52E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1299,7 +1485,7 @@
         <v>4269.8</v>
       </c>
       <c r="E11" s="4">
-        <v>4269.8</v>
+        <v>1384.8</v>
       </c>
       <c r="F11" s="4">
         <v>1384.8</v>
@@ -1310,8 +1496,26 @@
       <c r="H11" s="4">
         <v>1384.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="4">
+        <v>4269.8</v>
+      </c>
+      <c r="J11" s="4">
+        <v>4269.8</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1384.8</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1384.8</v>
+      </c>
+      <c r="M11" s="4">
+        <v>1384.8</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1384.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>101</v>
       </c>
@@ -1325,7 +1529,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
       <c r="E12" s="4">
-        <v>1.6999999999999999E-3</v>
+        <v>1.2E-4</v>
       </c>
       <c r="F12" s="4">
         <v>1.2E-4</v>
@@ -1336,8 +1540,26 @@
       <c r="H12" s="4">
         <v>1.2E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="4">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1.2E-4</v>
+      </c>
+      <c r="L12" s="4">
+        <v>1.2E-4</v>
+      </c>
+      <c r="M12" s="4">
+        <v>1.2E-4</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1.2E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1362,8 +1584,26 @@
       <c r="H13" s="4">
         <v>2.9999999999999997E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="J13" s="4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="M13" s="4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="N13" s="4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1388,8 +1628,26 @@
       <c r="H14" s="4">
         <v>1.8000000000000001E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="J14" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="K14" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="M14" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="N14" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>10</v>
       </c>
@@ -1414,8 +1672,26 @@
       <c r="H15" s="4">
         <v>4.8000000000000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="J15" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="K15" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="L15" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="M15" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="N15" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>11</v>
       </c>
@@ -1440,8 +1716,26 @@
       <c r="H16" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="J16" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="K16" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="L16" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="M16" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N16" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
@@ -1466,8 +1760,26 @@
       <c r="H17" s="4">
         <v>8.3999999999999995E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="4">
+        <v>8.3999999999999995E-5</v>
+      </c>
+      <c r="J17" s="4">
+        <v>8.3999999999999995E-5</v>
+      </c>
+      <c r="K17" s="4">
+        <v>8.3999999999999995E-5</v>
+      </c>
+      <c r="L17" s="4">
+        <v>8.3999999999999995E-5</v>
+      </c>
+      <c r="M17" s="4">
+        <v>8.3999999999999995E-5</v>
+      </c>
+      <c r="N17" s="4">
+        <v>8.3999999999999995E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1492,8 +1804,26 @@
       <c r="H18" s="4">
         <v>3.6000000000000001E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="J18" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="K18" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="L18" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="M18" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="N18" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>14</v>
       </c>
@@ -1518,8 +1848,26 @@
       <c r="H19" s="4">
         <v>1.08E-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="4">
+        <v>1.08E-4</v>
+      </c>
+      <c r="J19" s="4">
+        <v>1.08E-4</v>
+      </c>
+      <c r="K19" s="4">
+        <v>1.08E-4</v>
+      </c>
+      <c r="L19" s="4">
+        <v>1.08E-4</v>
+      </c>
+      <c r="M19" s="4">
+        <v>1.08E-4</v>
+      </c>
+      <c r="N19" s="4">
+        <v>1.08E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
@@ -1544,8 +1892,26 @@
       <c r="H20" s="4">
         <v>1.44E-4</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="4">
+        <v>1.44E-4</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1.44E-4</v>
+      </c>
+      <c r="K20" s="4">
+        <v>1.44E-4</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1.44E-4</v>
+      </c>
+      <c r="M20" s="4">
+        <v>1.44E-4</v>
+      </c>
+      <c r="N20" s="4">
+        <v>1.44E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -1570,8 +1936,26 @@
       <c r="H21" s="4">
         <v>9.6000000000000002E-5</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="J21" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="K21" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="L21" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="M21" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="N21" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -1596,8 +1980,26 @@
       <c r="H22" s="4">
         <v>9.6000000000000002E-5</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="J22" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="K22" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="L22" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="M22" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="N22" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>18</v>
       </c>
@@ -1622,8 +2024,26 @@
       <c r="H23" s="4">
         <v>9.6000000000000002E-5</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="J23" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="K23" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="L23" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="M23" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="N23" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>19</v>
       </c>
@@ -1648,8 +2068,26 @@
       <c r="H24" s="4">
         <v>1.6799999999999999E-4</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="4">
+        <v>1.6799999999999999E-4</v>
+      </c>
+      <c r="J24" s="4">
+        <v>1.6799999999999999E-4</v>
+      </c>
+      <c r="K24" s="4">
+        <v>1.6799999999999999E-4</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1.6799999999999999E-4</v>
+      </c>
+      <c r="M24" s="4">
+        <v>1.6799999999999999E-4</v>
+      </c>
+      <c r="N24" s="4">
+        <v>1.6799999999999999E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>20</v>
       </c>
@@ -1674,8 +2112,26 @@
       <c r="H25" s="4">
         <v>1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J25" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="K25" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="L25" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="M25" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="N25" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>21</v>
       </c>
@@ -1700,8 +2156,26 @@
       <c r="H26" s="4">
         <v>4.8000000000000001E-5</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I26" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="J26" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="K26" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="L26" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="M26" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="N26" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>22</v>
       </c>
@@ -1726,8 +2200,26 @@
       <c r="H27" s="4">
         <v>9.6000000000000002E-5</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="J27" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="K27" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="L27" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+      <c r="M27" s="4">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="N27" s="4">
+        <v>9.6000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>23</v>
       </c>
@@ -1752,8 +2244,26 @@
       <c r="H28" s="4">
         <v>3.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I28" s="4">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="J28" s="4">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="K28" s="4">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="L28" s="4">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="M28" s="4">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="N28" s="4">
+        <v>3.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>142</v>
       </c>
@@ -1778,8 +2288,26 @@
       <c r="H29" s="4">
         <v>5.9999999999999995E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I29" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="J29" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="K29" s="4">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="L29" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="M29" s="4">
+        <v>3.3E-3</v>
+      </c>
+      <c r="N29" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>24</v>
       </c>
@@ -1804,8 +2332,26 @@
       <c r="H30" s="4">
         <v>1.92E-4</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I30" s="4">
+        <v>1.92E-4</v>
+      </c>
+      <c r="J30" s="4">
+        <v>1.92E-4</v>
+      </c>
+      <c r="K30" s="4">
+        <v>1.92E-4</v>
+      </c>
+      <c r="L30" s="4">
+        <v>1.92E-4</v>
+      </c>
+      <c r="M30" s="4">
+        <v>1.92E-4</v>
+      </c>
+      <c r="N30" s="4">
+        <v>1.92E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
@@ -1830,8 +2376,26 @@
       <c r="H31" s="4">
         <v>4.2999999999999999E-4</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I31" s="4">
+        <v>4.2999999999999999E-4</v>
+      </c>
+      <c r="J31" s="4">
+        <v>4.2999999999999999E-4</v>
+      </c>
+      <c r="K31" s="4">
+        <v>2.3E-3</v>
+      </c>
+      <c r="L31" s="4">
+        <v>4.2999999999999999E-4</v>
+      </c>
+      <c r="M31" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="N31" s="4">
+        <v>4.2999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>26</v>
       </c>
@@ -1856,8 +2420,26 @@
       <c r="H32" s="4">
         <v>1.1000000000000001E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I32" s="4">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="J32" s="4">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="K32" s="4">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="M32" s="4">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="N32" s="4">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>27</v>
       </c>
@@ -1882,8 +2464,26 @@
       <c r="H33" s="4">
         <v>1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I33" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J33" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="K33" s="4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="L33" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="M33" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N33" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>28</v>
       </c>
@@ -1908,8 +2508,26 @@
       <c r="H34" s="4">
         <v>1.2E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I34" s="4">
+        <v>1.4E-2</v>
+      </c>
+      <c r="J34" s="4">
+        <v>1.2E-2</v>
+      </c>
+      <c r="K34" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L34" s="4">
+        <v>1.2E-2</v>
+      </c>
+      <c r="M34" s="4">
+        <v>1.2E-2</v>
+      </c>
+      <c r="N34" s="4">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>29</v>
       </c>
@@ -1934,8 +2552,26 @@
       <c r="H35" s="4">
         <v>2.7E-4</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I35" s="4">
+        <v>2.7E-4</v>
+      </c>
+      <c r="J35" s="4">
+        <v>2.7E-4</v>
+      </c>
+      <c r="K35" s="4">
+        <v>2.7E-4</v>
+      </c>
+      <c r="L35" s="4">
+        <v>2.7E-4</v>
+      </c>
+      <c r="M35" s="4">
+        <v>2.7E-4</v>
+      </c>
+      <c r="N35" s="4">
+        <v>2.7E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>30</v>
       </c>
@@ -1960,8 +2596,26 @@
       <c r="H36" s="4">
         <v>2.4000000000000001E-5</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I36" s="4">
+        <v>2.4000000000000001E-5</v>
+      </c>
+      <c r="J36" s="4">
+        <v>2.4000000000000001E-5</v>
+      </c>
+      <c r="K36" s="4">
+        <v>2.4000000000000001E-5</v>
+      </c>
+      <c r="L36" s="4">
+        <v>2.4000000000000001E-5</v>
+      </c>
+      <c r="M36" s="4">
+        <v>2.4000000000000001E-5</v>
+      </c>
+      <c r="N36" s="4">
+        <v>2.4000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>31</v>
       </c>
@@ -1975,7 +2629,7 @@
         <v>1.225E-3</v>
       </c>
       <c r="E37" s="4">
-        <v>1.225E-3</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="F37" s="4">
         <v>5.9999999999999995E-4</v>
@@ -1986,8 +2640,26 @@
       <c r="H37" s="4">
         <v>5.9999999999999995E-4</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I37" s="4">
+        <v>1.225E-3</v>
+      </c>
+      <c r="J37" s="4">
+        <v>1.225E-3</v>
+      </c>
+      <c r="K37" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="L37" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="M37" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="N37" s="4">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>32</v>
       </c>
@@ -2012,8 +2684,26 @@
       <c r="H38" s="4">
         <v>1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I38" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J38" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="K38" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="L38" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="M38" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="N38" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>33</v>
       </c>
@@ -2027,19 +2717,37 @@
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="E39" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="F39" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="G39" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="H39" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="I39" s="4">
         <v>4.8999999999999998E-4</v>
       </c>
-      <c r="F39" s="4">
-        <v>2.4000000000000001E-4</v>
-      </c>
-      <c r="G39" s="4">
-        <v>2.4000000000000001E-4</v>
-      </c>
-      <c r="H39" s="4">
-        <v>2.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J39" s="4">
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="K39" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="L39" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="M39" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N39" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>34</v>
       </c>
@@ -2053,7 +2761,7 @@
         <v>7.3499999999999998E-4</v>
       </c>
       <c r="E40" s="4">
-        <v>7.3499999999999998E-4</v>
+        <v>3.6000000000000002E-4</v>
       </c>
       <c r="F40" s="4">
         <v>3.6000000000000002E-4</v>
@@ -2064,8 +2772,26 @@
       <c r="H40" s="4">
         <v>3.6000000000000002E-4</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="4">
+        <v>7.3499999999999998E-4</v>
+      </c>
+      <c r="J40" s="4">
+        <v>7.3499999999999998E-4</v>
+      </c>
+      <c r="K40" s="4">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="L40" s="4">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="M40" s="4">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="N40" s="4">
+        <v>3.6000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>35</v>
       </c>
@@ -2079,19 +2805,37 @@
         <v>4.8999999999999998E-4</v>
       </c>
       <c r="E41" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="F41" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="G41" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="H41" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="I41" s="4">
         <v>4.8999999999999998E-4</v>
       </c>
-      <c r="F41" s="4">
-        <v>2.4000000000000001E-4</v>
-      </c>
-      <c r="G41" s="4">
-        <v>2.4000000000000001E-4</v>
-      </c>
-      <c r="H41" s="4">
-        <v>2.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J41" s="4">
+        <v>4.8999999999999998E-4</v>
+      </c>
+      <c r="K41" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="L41" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="M41" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N41" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>36</v>
       </c>
@@ -2116,8 +2860,26 @@
       <c r="H42" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I42" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="J42" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="K42" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="L42" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="M42" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N42" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>37</v>
       </c>
@@ -2142,8 +2904,26 @@
       <c r="H43" s="4">
         <v>2.7599999999999999E-4</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I43" s="4">
+        <v>2.7599999999999999E-4</v>
+      </c>
+      <c r="J43" s="4">
+        <v>2.7599999999999999E-4</v>
+      </c>
+      <c r="K43" s="4">
+        <v>2.7599999999999999E-4</v>
+      </c>
+      <c r="L43" s="4">
+        <v>2.7599999999999999E-4</v>
+      </c>
+      <c r="M43" s="4">
+        <v>2.7599999999999999E-4</v>
+      </c>
+      <c r="N43" s="4">
+        <v>2.7599999999999999E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>38</v>
       </c>
@@ -2157,19 +2937,37 @@
         <v>6.6500000000000001E-4</v>
       </c>
       <c r="E44" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="F44" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="G44" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="H44" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="I44" s="4">
         <v>6.6500000000000001E-4</v>
       </c>
-      <c r="F44" s="4">
-        <v>2.4000000000000001E-4</v>
-      </c>
-      <c r="G44" s="4">
-        <v>2.4000000000000001E-4</v>
-      </c>
-      <c r="H44" s="4">
-        <v>2.4000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="J44" s="4">
+        <v>6.6500000000000001E-4</v>
+      </c>
+      <c r="K44" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="L44" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="M44" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N44" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>39</v>
       </c>
@@ -2183,7 +2981,7 @@
         <v>3.2000000000000003E-4</v>
       </c>
       <c r="E45" s="4">
-        <v>3.2000000000000003E-4</v>
+        <v>1.2E-4</v>
       </c>
       <c r="F45" s="4">
         <v>1.2E-4</v>
@@ -2194,8 +2992,26 @@
       <c r="H45" s="4">
         <v>1.2E-4</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I45" s="4">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="J45" s="4">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="K45" s="4">
+        <v>1.2E-4</v>
+      </c>
+      <c r="L45" s="4">
+        <v>1.2E-4</v>
+      </c>
+      <c r="M45" s="4">
+        <v>1.2E-4</v>
+      </c>
+      <c r="N45" s="4">
+        <v>1.2E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>40</v>
       </c>
@@ -2220,8 +3036,26 @@
       <c r="H46" s="4">
         <v>2.16E-5</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I46" s="4">
+        <v>2.16E-5</v>
+      </c>
+      <c r="J46" s="4">
+        <v>2.16E-5</v>
+      </c>
+      <c r="K46" s="4">
+        <v>2.16E-5</v>
+      </c>
+      <c r="L46" s="4">
+        <v>2.16E-5</v>
+      </c>
+      <c r="M46" s="4">
+        <v>2.16E-5</v>
+      </c>
+      <c r="N46" s="4">
+        <v>2.16E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>41</v>
       </c>
@@ -2246,8 +3080,26 @@
       <c r="H47" s="4">
         <v>1.8000000000000001E-4</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I47" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="J47" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="K47" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="L47" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="M47" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="N47" s="4">
+        <v>1.8000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>42</v>
       </c>
@@ -2272,8 +3124,26 @@
       <c r="H48" s="4">
         <v>6.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I48" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="J48" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="K48" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="L48" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="M48" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="N48" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>43</v>
       </c>
@@ -2298,8 +3168,26 @@
       <c r="H49" s="4">
         <v>3.6000000000000001E-5</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I49" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="J49" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="K49" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="L49" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="M49" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="N49" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>44</v>
       </c>
@@ -2324,8 +3212,26 @@
       <c r="H50" s="4">
         <v>3.6000000000000001E-5</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="J50" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="K50" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="L50" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="M50" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="N50" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>45</v>
       </c>
@@ -2350,8 +3256,26 @@
       <c r="H51" s="4">
         <v>6.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I51" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="J51" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="K51" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="L51" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="M51" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="N51" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>144</v>
       </c>
@@ -2376,8 +3300,26 @@
       <c r="H52" s="4">
         <v>3.6000000000000001E-5</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="J52" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="K52" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="L52" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="M52" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="N52" s="4">
+        <v>3.6000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
         <v>47</v>
       </c>
@@ -2402,8 +3344,26 @@
       <c r="H53" s="4">
         <v>4.8000000000000001E-5</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="J53" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="K53" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="L53" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="M53" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="N53" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>46</v>
       </c>
@@ -2428,8 +3388,26 @@
       <c r="H54" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I54" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="J54" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="K54" s="4">
+        <v>6.8000000000000005E-4</v>
+      </c>
+      <c r="L54" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="M54" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+      <c r="N54" s="4">
+        <v>2.4000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>48</v>
       </c>
@@ -2454,8 +3432,26 @@
       <c r="H55" s="4">
         <v>4.8000000000000001E-4</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I55" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="J55" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="K55" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="L55" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="M55" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+      <c r="N55" s="4">
+        <v>4.8000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>49</v>
       </c>
@@ -2480,8 +3476,26 @@
       <c r="H56" s="4">
         <v>6.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I56" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="J56" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="K56" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="L56" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="M56" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="N56" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>30</v>
       </c>
@@ -2506,8 +3520,26 @@
       <c r="H57" s="4">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I57" s="4">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="J57" s="4">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="K57" s="4">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="L57" s="4">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="M57" s="4">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="N57" s="4">
+        <v>1.4999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>50</v>
       </c>
@@ -2532,8 +3564,26 @@
       <c r="H58" s="4">
         <v>2.8799999999999999E-5</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" s="4">
+        <v>2.8799999999999999E-5</v>
+      </c>
+      <c r="J58" s="4">
+        <v>2.8799999999999999E-5</v>
+      </c>
+      <c r="K58" s="4">
+        <v>2.8799999999999999E-5</v>
+      </c>
+      <c r="L58" s="4">
+        <v>2.8799999999999999E-5</v>
+      </c>
+      <c r="M58" s="4">
+        <v>2.8799999999999999E-5</v>
+      </c>
+      <c r="N58" s="4">
+        <v>2.8799999999999999E-5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
         <v>51</v>
       </c>
@@ -2558,8 +3608,26 @@
       <c r="H59" s="4">
         <v>1.56E-5</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" s="4">
+        <v>1.56E-5</v>
+      </c>
+      <c r="J59" s="4">
+        <v>1.56E-5</v>
+      </c>
+      <c r="K59" s="4">
+        <v>1.56E-5</v>
+      </c>
+      <c r="L59" s="4">
+        <v>1.56E-5</v>
+      </c>
+      <c r="M59" s="4">
+        <v>1.56E-5</v>
+      </c>
+      <c r="N59" s="4">
+        <v>1.56E-5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
         <v>52</v>
       </c>
@@ -2584,8 +3652,26 @@
       <c r="H60" s="4">
         <v>1.91E-5</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" s="4">
+        <v>1.91E-5</v>
+      </c>
+      <c r="J60" s="4">
+        <v>1.91E-5</v>
+      </c>
+      <c r="K60" s="4">
+        <v>1.91E-5</v>
+      </c>
+      <c r="L60" s="4">
+        <v>1.91E-5</v>
+      </c>
+      <c r="M60" s="4">
+        <v>1.91E-5</v>
+      </c>
+      <c r="N60" s="4">
+        <v>1.91E-5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
         <v>53</v>
       </c>
@@ -2610,8 +3696,26 @@
       <c r="H61" s="4">
         <v>4.6099999999999999E-6</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I61" s="4">
+        <v>4.6099999999999999E-6</v>
+      </c>
+      <c r="J61" s="4">
+        <v>4.6099999999999999E-6</v>
+      </c>
+      <c r="K61" s="4">
+        <v>4.6099999999999999E-6</v>
+      </c>
+      <c r="L61" s="4">
+        <v>4.6099999999999999E-6</v>
+      </c>
+      <c r="M61" s="4">
+        <v>4.6099999999999999E-6</v>
+      </c>
+      <c r="N61" s="4">
+        <v>4.6099999999999999E-6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
         <v>54</v>
       </c>
@@ -2636,8 +3740,26 @@
       <c r="H62" s="4">
         <v>3.3699999999999999E-5</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" s="4">
+        <v>3.3699999999999999E-5</v>
+      </c>
+      <c r="J62" s="4">
+        <v>3.3699999999999999E-5</v>
+      </c>
+      <c r="K62" s="4">
+        <v>3.3699999999999999E-5</v>
+      </c>
+      <c r="L62" s="4">
+        <v>3.3699999999999999E-5</v>
+      </c>
+      <c r="M62" s="4">
+        <v>3.3699999999999999E-5</v>
+      </c>
+      <c r="N62" s="4">
+        <v>3.3699999999999999E-5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
         <v>55</v>
       </c>
@@ -2662,8 +3784,26 @@
       <c r="H63" s="4">
         <v>3.79E-5</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" s="4">
+        <v>3.79E-5</v>
+      </c>
+      <c r="J63" s="4">
+        <v>3.79E-5</v>
+      </c>
+      <c r="K63" s="4">
+        <v>3.79E-5</v>
+      </c>
+      <c r="L63" s="4">
+        <v>3.79E-5</v>
+      </c>
+      <c r="M63" s="4">
+        <v>3.79E-5</v>
+      </c>
+      <c r="N63" s="4">
+        <v>3.79E-5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
         <v>56</v>
       </c>
@@ -2688,8 +3828,26 @@
       <c r="H64" s="4">
         <v>5.94E-5</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" s="4">
+        <v>5.94E-5</v>
+      </c>
+      <c r="J64" s="4">
+        <v>5.94E-5</v>
+      </c>
+      <c r="K64" s="4">
+        <v>5.94E-5</v>
+      </c>
+      <c r="L64" s="4">
+        <v>5.94E-5</v>
+      </c>
+      <c r="M64" s="4">
+        <v>5.94E-5</v>
+      </c>
+      <c r="N64" s="4">
+        <v>5.94E-5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
         <v>57</v>
       </c>
@@ -2714,8 +3872,26 @@
       <c r="H65" s="4">
         <v>1.5800000000000001E-5</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" s="4">
+        <v>1.5800000000000001E-5</v>
+      </c>
+      <c r="J65" s="4">
+        <v>1.5800000000000001E-5</v>
+      </c>
+      <c r="K65" s="4">
+        <v>1.5800000000000001E-5</v>
+      </c>
+      <c r="L65" s="4">
+        <v>1.5800000000000001E-5</v>
+      </c>
+      <c r="M65" s="4">
+        <v>1.5800000000000001E-5</v>
+      </c>
+      <c r="N65" s="4">
+        <v>1.5800000000000001E-5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
         <v>58</v>
       </c>
@@ -2740,8 +3916,26 @@
       <c r="H66" s="4">
         <v>2.3300000000000001E-5</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" s="4">
+        <v>2.3300000000000001E-5</v>
+      </c>
+      <c r="J66" s="4">
+        <v>2.3300000000000001E-5</v>
+      </c>
+      <c r="K66" s="4">
+        <v>2.3300000000000001E-5</v>
+      </c>
+      <c r="L66" s="4">
+        <v>2.3300000000000001E-5</v>
+      </c>
+      <c r="M66" s="4">
+        <v>2.3300000000000001E-5</v>
+      </c>
+      <c r="N66" s="4">
+        <v>2.3300000000000001E-5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
         <v>59</v>
       </c>
@@ -2766,8 +3960,26 @@
       <c r="H67" s="4">
         <v>8.7999999999999998E-5</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I67" s="4">
+        <v>8.7999999999999998E-5</v>
+      </c>
+      <c r="J67" s="4">
+        <v>8.7999999999999998E-5</v>
+      </c>
+      <c r="K67" s="4">
+        <v>8.7999999999999998E-5</v>
+      </c>
+      <c r="L67" s="4">
+        <v>8.7999999999999998E-5</v>
+      </c>
+      <c r="M67" s="4">
+        <v>8.7999999999999998E-5</v>
+      </c>
+      <c r="N67" s="4">
+        <v>8.7999999999999998E-5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
         <v>60</v>
       </c>
@@ -2792,8 +4004,26 @@
       <c r="H68" s="4">
         <v>2.5700000000000001E-5</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I68" s="4">
+        <v>2.5700000000000001E-5</v>
+      </c>
+      <c r="J68" s="4">
+        <v>2.5700000000000001E-5</v>
+      </c>
+      <c r="K68" s="4">
+        <v>2.5700000000000001E-5</v>
+      </c>
+      <c r="L68" s="4">
+        <v>2.5700000000000001E-5</v>
+      </c>
+      <c r="M68" s="4">
+        <v>2.5700000000000001E-5</v>
+      </c>
+      <c r="N68" s="4">
+        <v>2.5700000000000001E-5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>151</v>
       </c>
@@ -2806,8 +4036,8 @@
       <c r="D69" s="4">
         <v>1.1E-5</v>
       </c>
-      <c r="E69" s="4">
-        <v>1.1E-5</v>
+      <c r="E69" s="16">
+        <v>5.8000000000000004E-6</v>
       </c>
       <c r="F69" s="16">
         <v>5.8000000000000004E-6</v>
@@ -2818,8 +4048,26 @@
       <c r="H69" s="16">
         <v>5.8000000000000004E-6</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" s="4">
+        <v>1.1E-5</v>
+      </c>
+      <c r="J69" s="4">
+        <v>1.1E-5</v>
+      </c>
+      <c r="K69" s="16">
+        <v>5.8000000000000004E-6</v>
+      </c>
+      <c r="L69" s="16">
+        <v>5.8000000000000004E-6</v>
+      </c>
+      <c r="M69" s="16">
+        <v>5.8000000000000004E-6</v>
+      </c>
+      <c r="N69" s="16">
+        <v>5.8000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>154</v>
       </c>
@@ -2833,7 +4081,7 @@
         <v>2.8600000000000001E-5</v>
       </c>
       <c r="E70" s="4">
-        <v>2.8600000000000001E-5</v>
+        <v>1.508E-5</v>
       </c>
       <c r="F70" s="4">
         <v>1.508E-5</v>
@@ -2844,8 +4092,26 @@
       <c r="H70" s="4">
         <v>1.508E-5</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" s="4">
+        <v>2.8600000000000001E-5</v>
+      </c>
+      <c r="J70" s="4">
+        <v>2.8600000000000001E-5</v>
+      </c>
+      <c r="K70" s="4">
+        <v>1.508E-5</v>
+      </c>
+      <c r="L70" s="4">
+        <v>1.508E-5</v>
+      </c>
+      <c r="M70" s="4">
+        <v>1.508E-5</v>
+      </c>
+      <c r="N70" s="4">
+        <v>1.508E-5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>48</v>
       </c>
@@ -2870,8 +4136,26 @@
       <c r="H71" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" s="2">
+        <v>4.1700000000000001E-3</v>
+      </c>
+      <c r="J71" s="4">
+        <v>0</v>
+      </c>
+      <c r="K71" s="4">
+        <v>0</v>
+      </c>
+      <c r="L71" s="4">
+        <v>0</v>
+      </c>
+      <c r="M71" s="4">
+        <v>0</v>
+      </c>
+      <c r="N71" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>157</v>
       </c>
@@ -2884,7 +4168,7 @@
       <c r="D72" s="4">
         <v>0</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="4">
         <v>0</v>
       </c>
       <c r="F72" s="4">
@@ -2896,8 +4180,26 @@
       <c r="H72" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" s="4">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="J72" s="4">
+        <v>0</v>
+      </c>
+      <c r="K72" s="4">
+        <v>0</v>
+      </c>
+      <c r="L72" s="4">
+        <v>0</v>
+      </c>
+      <c r="M72" s="4">
+        <v>0</v>
+      </c>
+      <c r="N72" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
         <v>160</v>
       </c>
@@ -2922,8 +4224,26 @@
       <c r="H73" s="4">
         <v>6.7200000000000003E-3</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I73" s="4">
+        <v>6.7200000000000003E-3</v>
+      </c>
+      <c r="J73" s="4">
+        <v>6.7200000000000003E-3</v>
+      </c>
+      <c r="K73" s="4">
+        <v>1.2E-2</v>
+      </c>
+      <c r="L73" s="4">
+        <v>6.7200000000000003E-3</v>
+      </c>
+      <c r="M73" s="4">
+        <v>6.7200000000000003E-3</v>
+      </c>
+      <c r="N73" s="4">
+        <v>6.7200000000000003E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
         <v>162</v>
       </c>
@@ -2948,8 +4268,26 @@
       <c r="H74" s="2">
         <v>1.4E-3</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="J74" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="K74" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="L74" s="2">
+        <v>1.4E-3</v>
+      </c>
+      <c r="M74" s="2">
+        <v>1.9E-3</v>
+      </c>
+      <c r="N74" s="2">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>171</v>
       </c>
@@ -2963,7 +4301,7 @@
         <v>0</v>
       </c>
       <c r="E75" s="2">
-        <v>8.4999999999999995E-4</v>
+        <v>0</v>
       </c>
       <c r="F75" s="2">
         <v>0</v>
@@ -2974,8 +4312,26 @@
       <c r="H75" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" s="2">
+        <v>0</v>
+      </c>
+      <c r="J75" s="2">
+        <v>0</v>
+      </c>
+      <c r="K75" s="2">
+        <v>0</v>
+      </c>
+      <c r="L75" s="2">
+        <v>0</v>
+      </c>
+      <c r="M75" s="2">
+        <v>0</v>
+      </c>
+      <c r="N75" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>173</v>
       </c>
@@ -2998,6 +4354,24 @@
         <v>0</v>
       </c>
       <c r="H76" s="2">
+        <v>0</v>
+      </c>
+      <c r="I76" s="2">
+        <v>0</v>
+      </c>
+      <c r="J76" s="2">
+        <v>0</v>
+      </c>
+      <c r="K76" s="2">
+        <v>6.3000000000000003E-4</v>
+      </c>
+      <c r="L76" s="2">
+        <v>0</v>
+      </c>
+      <c r="M76" s="2">
+        <v>0</v>
+      </c>
+      <c r="N76" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3008,10 +4382,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E43D553-2DA6-5946-9E4C-D6464FED6905}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3717,81 +5091,80 @@
       <c r="F65" s="16"/>
     </row>
     <row r="66" spans="4:6" ht="38" x14ac:dyDescent="0.2">
-      <c r="D66" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="E66" s="17" t="s">
-        <v>48</v>
+      <c r="D66" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="F66" s="16"/>
     </row>
-    <row r="67" spans="4:6" ht="38" x14ac:dyDescent="0.2">
-      <c r="D67" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>157</v>
-      </c>
+    <row r="67" spans="4:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="D67" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="E67" s="17"/>
       <c r="F67" s="16"/>
     </row>
     <row r="68" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D68" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="E68" s="17"/>
+        <v>159</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>160</v>
+      </c>
       <c r="F68" s="16"/>
     </row>
     <row r="69" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D69" s="18" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F69" s="16"/>
     </row>
     <row r="70" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D70" s="18" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="F70" s="16"/>
     </row>
     <row r="71" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D71" s="18" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E71" s="10" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F71" s="16"/>
     </row>
     <row r="72" spans="4:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="D72" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>173</v>
-      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="17"/>
       <c r="F72" s="16"/>
     </row>
     <row r="73" spans="4:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="D73" s="18"/>
-      <c r="E73" s="17"/>
+      <c r="D73" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="E73" s="19"/>
       <c r="F73" s="16"/>
     </row>
     <row r="74" spans="4:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="D74" s="20" t="s">
+      <c r="D74" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E74" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E74" s="19"/>
-      <c r="F74" s="16"/>
     </row>
     <row r="75" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D75" s="11" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>141</v>
@@ -3799,15 +5172,15 @@
     </row>
     <row r="76" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D76" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="77" spans="4:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="D77" s="11" t="s">
-        <v>116</v>
+      <c r="D77" t="s">
+        <v>140</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>141</v>
@@ -3815,7 +5188,7 @@
     </row>
     <row r="78" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D78" t="s">
-        <v>140</v>
+        <v>67</v>
       </c>
       <c r="E78" s="10" t="s">
         <v>141</v>
@@ -3823,7 +5196,7 @@
     </row>
     <row r="79" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D79" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>141</v>
@@ -3831,7 +5204,7 @@
     </row>
     <row r="80" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D80" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E80" s="10" t="s">
         <v>141</v>
@@ -3839,7 +5212,7 @@
     </row>
     <row r="81" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D81" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E81" s="10" t="s">
         <v>141</v>
@@ -3847,7 +5220,7 @@
     </row>
     <row r="82" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D82" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E82" s="10" t="s">
         <v>141</v>
@@ -3855,7 +5228,7 @@
     </row>
     <row r="83" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D83" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E83" s="10" t="s">
         <v>141</v>
@@ -3863,7 +5236,7 @@
     </row>
     <row r="84" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D84" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E84" s="10" t="s">
         <v>141</v>
@@ -3871,7 +5244,7 @@
     </row>
     <row r="85" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>141</v>
@@ -3879,7 +5252,7 @@
     </row>
     <row r="86" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D86" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E86" s="10" t="s">
         <v>141</v>
@@ -3887,7 +5260,7 @@
     </row>
     <row r="87" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D87" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>141</v>
@@ -3895,7 +5268,7 @@
     </row>
     <row r="88" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E88" s="10" t="s">
         <v>141</v>
@@ -3903,7 +5276,7 @@
     </row>
     <row r="89" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
-        <v>94</v>
+        <v>163</v>
       </c>
       <c r="E89" s="10" t="s">
         <v>141</v>
@@ -3911,15 +5284,15 @@
     </row>
     <row r="90" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D90" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E90" s="10" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="91" spans="4:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="D91" t="s">
-        <v>164</v>
+      <c r="D91" s="18" t="s">
+        <v>165</v>
       </c>
       <c r="E91" s="10" t="s">
         <v>141</v>
@@ -3927,7 +5300,7 @@
     </row>
     <row r="92" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D92" s="18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E92" s="10" t="s">
         <v>141</v>
@@ -3935,7 +5308,7 @@
     </row>
     <row r="93" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D93" s="18" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>141</v>
@@ -3943,31 +5316,23 @@
     </row>
     <row r="94" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D94" s="18" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E94" s="10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="95" spans="4:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="D95" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D97" s="12" t="s">
+    <row r="96" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D96" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="E97" s="12"/>
-    </row>
-    <row r="98" spans="4:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="D98" s="21" t="s">
+      <c r="E96" s="12"/>
+    </row>
+    <row r="97" spans="4:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="D97" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="E98" s="10" t="s">
+      <c r="E97" s="10" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
better dealing with input xlsx
better interpretation of xlsx files containing influxes and wall loss rate coefficients
</commit_message>
<xml_diff>
--- a/PyCHAM/input/ind_AQ_ex/const_infl.xlsx
+++ b/PyCHAM/input/ind_AQ_ex/const_infl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Psymo\Desktop\PyCHAM\PyCHAM\PyCHAM\input\ind_AQ_ex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/GitHub/PyCHAM/PyCHAM/input/ind_AQ_ex/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A10F154-101F-49C8-B2B4-E0D9FC2A2D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE0503C-7182-FB45-A349-EF960A942BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="84" yWindow="1392" windowWidth="22380" windowHeight="10560" xr2:uid="{A12B527E-AFAD-6348-8F8E-CC39D59E777A}"/>
+    <workbookView xWindow="80" yWindow="1400" windowWidth="32260" windowHeight="16380" xr2:uid="{A12B527E-AFAD-6348-8F8E-CC39D59E777A}"/>
   </bookViews>
   <sheets>
     <sheet name="const_infl" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="176">
   <si>
     <t>CO</t>
   </si>
@@ -562,6 +562,9 @@
   </si>
   <si>
     <t>ppb</t>
+  </si>
+  <si>
+    <t>CH3CHO</t>
   </si>
 </sst>
 </file>
@@ -572,7 +575,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -613,6 +616,24 @@
       <sz val="13.5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -672,7 +693,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -704,6 +725,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1019,26 +1045,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9915D14-D182-E247-B384-ACBF32C9043F}">
-  <dimension ref="A1:N76"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="18.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.296875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
-    <col min="11" max="11" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="12.796875" customWidth="1"/>
-    <col min="14" max="14" width="14.19921875" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>174</v>
       </c>
@@ -1081,8 +1111,13 @@
       <c r="N1" s="16">
         <v>159300</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="4">
+        <f>E1-F1</f>
+        <v>-1200</v>
+      </c>
+      <c r="P1" s="4"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1125,8 +1160,12 @@
       <c r="N2" s="4">
         <v>4.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="4">
+        <f t="shared" ref="O2:O65" si="0">F2-E2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1169,8 +1208,12 @@
       <c r="N3" s="7">
         <v>0.22800000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="O3" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1213,8 +1256,12 @@
       <c r="N4" s="4">
         <v>1.032E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="O4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1257,8 +1304,12 @@
       <c r="N5" s="4">
         <v>7.0200000000000004E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="O5" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1301,8 +1352,12 @@
       <c r="N6" s="8">
         <v>5.1599999999999997E-4</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1345,8 +1400,12 @@
       <c r="N7" s="4">
         <v>1.1039999999999999E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
@@ -1389,8 +1448,12 @@
       <c r="N8" s="4">
         <v>1.1999999999999999E-6</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>61</v>
       </c>
@@ -1433,8 +1496,12 @@
       <c r="N9" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>62</v>
       </c>
@@ -1477,8 +1544,12 @@
       <c r="N10" s="4">
         <v>8.52E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1521,8 +1592,12 @@
       <c r="N11" s="4">
         <v>1384.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>100</v>
       </c>
@@ -1565,8 +1640,12 @@
       <c r="N12" s="4">
         <v>1.2E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
@@ -1609,8 +1688,12 @@
       <c r="N13" s="4">
         <v>2.9999999999999997E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="O13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -1653,8 +1736,12 @@
       <c r="N14" s="4">
         <v>1.8000000000000001E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
         <v>9</v>
       </c>
@@ -1697,8 +1784,12 @@
       <c r="N15" s="4">
         <v>4.8000000000000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
         <v>10</v>
       </c>
@@ -1741,8 +1832,12 @@
       <c r="N16" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1785,8 +1880,12 @@
       <c r="N17" s="4">
         <v>8.3999999999999995E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="O17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -1829,8 +1928,12 @@
       <c r="N18" s="4">
         <v>3.6000000000000001E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="O18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>13</v>
       </c>
@@ -1873,8 +1976,12 @@
       <c r="N19" s="4">
         <v>1.08E-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
@@ -1917,8 +2024,12 @@
       <c r="N20" s="4">
         <v>1.44E-4</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="O20" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
@@ -1961,8 +2072,12 @@
       <c r="N21" s="4">
         <v>9.6000000000000002E-5</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="O21" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -2005,8 +2120,12 @@
       <c r="N22" s="4">
         <v>9.6000000000000002E-5</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="O22" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>17</v>
       </c>
@@ -2049,8 +2168,12 @@
       <c r="N23" s="4">
         <v>9.6000000000000002E-5</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="O23" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
@@ -2093,8 +2216,12 @@
       <c r="N24" s="4">
         <v>1.6799999999999999E-4</v>
       </c>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="O24" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
         <v>19</v>
       </c>
@@ -2137,8 +2264,12 @@
       <c r="N25" s="4">
         <v>1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="O25" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
         <v>20</v>
       </c>
@@ -2181,8 +2312,12 @@
       <c r="N26" s="4">
         <v>4.8000000000000001E-5</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="O26" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>21</v>
       </c>
@@ -2225,9 +2360,13 @@
       <c r="N27" s="4">
         <v>9.6000000000000002E-5</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="3" t="s">
+      <c r="O27" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="4">
@@ -2269,10 +2408,14 @@
       <c r="N28" s="4">
         <v>3.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="5" t="s">
-        <v>141</v>
+      <c r="O28" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
+        <v>175</v>
       </c>
       <c r="B29" s="4">
         <v>5.9999999999999995E-4</v>
@@ -2313,9 +2456,13 @@
       <c r="N29" s="4">
         <v>5.9999999999999995E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="5" t="s">
+      <c r="O29" s="4">
+        <f t="shared" si="0"/>
+        <v>-3.3E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="4">
@@ -2357,8 +2504,12 @@
       <c r="N30" s="4">
         <v>1.92E-4</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="O30" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>24</v>
       </c>
@@ -2401,8 +2552,12 @@
       <c r="N31" s="4">
         <v>4.2999999999999999E-4</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="O31" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.8699999999999999E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
@@ -2445,8 +2600,12 @@
       <c r="N32" s="4">
         <v>1.1000000000000001E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="O32" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>26</v>
       </c>
@@ -2489,8 +2648,12 @@
       <c r="N33" s="4">
         <v>1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="O33" s="4">
+        <f t="shared" si="0"/>
+        <v>-1.18E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>27</v>
       </c>
@@ -2533,8 +2696,12 @@
       <c r="N34" s="4">
         <v>1.2E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="O34" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>28</v>
       </c>
@@ -2577,8 +2744,12 @@
       <c r="N35" s="4">
         <v>2.7E-4</v>
       </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="O35" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>29</v>
       </c>
@@ -2621,8 +2792,12 @@
       <c r="N36" s="4">
         <v>2.4000000000000001E-5</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="O36" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>30</v>
       </c>
@@ -2665,8 +2840,12 @@
       <c r="N37" s="4">
         <v>5.9999999999999995E-4</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="O37" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>31</v>
       </c>
@@ -2709,8 +2888,12 @@
       <c r="N38" s="4">
         <v>1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="O38" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>32</v>
       </c>
@@ -2753,8 +2936,12 @@
       <c r="N39" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="O39" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>33</v>
       </c>
@@ -2797,8 +2984,12 @@
       <c r="N40" s="4">
         <v>3.6000000000000002E-4</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="O40" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -2841,8 +3032,12 @@
       <c r="N41" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="O41" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>35</v>
       </c>
@@ -2885,8 +3080,12 @@
       <c r="N42" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="O42" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>36</v>
       </c>
@@ -2929,8 +3128,12 @@
       <c r="N43" s="4">
         <v>2.7599999999999999E-4</v>
       </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="O43" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
         <v>37</v>
       </c>
@@ -2973,8 +3176,12 @@
       <c r="N44" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="O44" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
         <v>38</v>
       </c>
@@ -3017,8 +3224,12 @@
       <c r="N45" s="4">
         <v>1.2E-4</v>
       </c>
-    </row>
-    <row r="46" spans="1:14">
+      <c r="O45" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
         <v>39</v>
       </c>
@@ -3061,8 +3272,12 @@
       <c r="N46" s="4">
         <v>2.16E-5</v>
       </c>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="O46" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>40</v>
       </c>
@@ -3105,8 +3320,12 @@
       <c r="N47" s="4">
         <v>1.8000000000000001E-4</v>
       </c>
-    </row>
-    <row r="48" spans="1:14">
+      <c r="O47" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>41</v>
       </c>
@@ -3149,8 +3368,12 @@
       <c r="N48" s="4">
         <v>6.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="O48" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>42</v>
       </c>
@@ -3193,8 +3416,12 @@
       <c r="N49" s="4">
         <v>3.6000000000000001E-5</v>
       </c>
-    </row>
-    <row r="50" spans="1:14">
+      <c r="O49" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>43</v>
       </c>
@@ -3237,8 +3464,12 @@
       <c r="N50" s="4">
         <v>3.6000000000000001E-5</v>
       </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="O50" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
         <v>44</v>
       </c>
@@ -3281,8 +3512,12 @@
       <c r="N51" s="4">
         <v>6.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="O51" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>143</v>
       </c>
@@ -3325,8 +3560,12 @@
       <c r="N52" s="4">
         <v>3.6000000000000001E-5</v>
       </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="O52" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
         <v>46</v>
       </c>
@@ -3369,8 +3608,12 @@
       <c r="N53" s="4">
         <v>4.8000000000000001E-5</v>
       </c>
-    </row>
-    <row r="54" spans="1:14">
+      <c r="O53" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
         <v>45</v>
       </c>
@@ -3413,8 +3656,12 @@
       <c r="N54" s="4">
         <v>2.4000000000000001E-4</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="O54" s="4">
+        <f t="shared" si="0"/>
+        <v>-4.4000000000000007E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>47</v>
       </c>
@@ -3457,8 +3704,12 @@
       <c r="N55" s="4">
         <v>4.8000000000000001E-4</v>
       </c>
-    </row>
-    <row r="56" spans="1:14">
+      <c r="O55" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>48</v>
       </c>
@@ -3501,8 +3752,12 @@
       <c r="N56" s="4">
         <v>6.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="57" spans="1:14">
+      <c r="O56" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>29</v>
       </c>
@@ -3545,8 +3800,12 @@
       <c r="N57" s="4">
         <v>1.4999999999999999E-4</v>
       </c>
-    </row>
-    <row r="58" spans="1:14">
+      <c r="O57" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>49</v>
       </c>
@@ -3589,8 +3848,12 @@
       <c r="N58" s="4">
         <v>2.8799999999999999E-5</v>
       </c>
-    </row>
-    <row r="59" spans="1:14">
+      <c r="O58" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
         <v>50</v>
       </c>
@@ -3633,8 +3896,12 @@
       <c r="N59" s="4">
         <v>1.56E-5</v>
       </c>
-    </row>
-    <row r="60" spans="1:14">
+      <c r="O59" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
         <v>51</v>
       </c>
@@ -3677,8 +3944,12 @@
       <c r="N60" s="4">
         <v>1.91E-5</v>
       </c>
-    </row>
-    <row r="61" spans="1:14">
+      <c r="O60" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
         <v>52</v>
       </c>
@@ -3721,8 +3992,12 @@
       <c r="N61" s="4">
         <v>4.6099999999999999E-6</v>
       </c>
-    </row>
-    <row r="62" spans="1:14">
+      <c r="O61" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
         <v>53</v>
       </c>
@@ -3765,8 +4040,12 @@
       <c r="N62" s="4">
         <v>3.3699999999999999E-5</v>
       </c>
-    </row>
-    <row r="63" spans="1:14">
+      <c r="O62" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
         <v>54</v>
       </c>
@@ -3809,8 +4088,12 @@
       <c r="N63" s="4">
         <v>3.79E-5</v>
       </c>
-    </row>
-    <row r="64" spans="1:14">
+      <c r="O63" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
         <v>55</v>
       </c>
@@ -3853,8 +4136,12 @@
       <c r="N64" s="4">
         <v>5.94E-5</v>
       </c>
-    </row>
-    <row r="65" spans="1:14">
+      <c r="O64" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
         <v>56</v>
       </c>
@@ -3897,8 +4184,12 @@
       <c r="N65" s="4">
         <v>1.5800000000000001E-5</v>
       </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="O65" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
         <v>57</v>
       </c>
@@ -3941,8 +4232,12 @@
       <c r="N66" s="4">
         <v>2.3300000000000001E-5</v>
       </c>
-    </row>
-    <row r="67" spans="1:14">
+      <c r="O66" s="4">
+        <f t="shared" ref="O66:O76" si="1">F66-E66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
         <v>58</v>
       </c>
@@ -3985,8 +4280,12 @@
       <c r="N67" s="4">
         <v>8.7999999999999998E-5</v>
       </c>
-    </row>
-    <row r="68" spans="1:14">
+      <c r="O67" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
         <v>59</v>
       </c>
@@ -4029,8 +4328,12 @@
       <c r="N68" s="4">
         <v>2.5700000000000001E-5</v>
       </c>
-    </row>
-    <row r="69" spans="1:14">
+      <c r="O68" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>150</v>
       </c>
@@ -4073,8 +4376,12 @@
       <c r="N69" s="16">
         <v>5.8000000000000004E-6</v>
       </c>
-    </row>
-    <row r="70" spans="1:14">
+      <c r="O69" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>152</v>
       </c>
@@ -4117,8 +4424,12 @@
       <c r="N70" s="4">
         <v>1.508E-5</v>
       </c>
-    </row>
-    <row r="71" spans="1:14">
+      <c r="O70" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>47</v>
       </c>
@@ -4161,8 +4472,12 @@
       <c r="N71" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:14">
+      <c r="O71" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="6" t="s">
         <v>154</v>
       </c>
@@ -4205,8 +4520,12 @@
       <c r="N72" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:14">
+      <c r="O72" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
         <v>156</v>
       </c>
@@ -4249,8 +4568,12 @@
       <c r="N73" s="4">
         <v>6.7200000000000003E-3</v>
       </c>
-    </row>
-    <row r="74" spans="1:14">
+      <c r="O73" s="4">
+        <f t="shared" si="1"/>
+        <v>-5.28E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
         <v>158</v>
       </c>
@@ -4293,8 +4616,12 @@
       <c r="N74" s="2">
         <v>1.4E-3</v>
       </c>
-    </row>
-    <row r="75" spans="1:14">
+      <c r="O74" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
         <v>167</v>
       </c>
@@ -4337,8 +4664,12 @@
       <c r="N75" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:14">
+      <c r="O75" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="6" t="s">
         <v>169</v>
       </c>
@@ -4380,6 +4711,10 @@
       </c>
       <c r="N76" s="2">
         <v>0</v>
+      </c>
+      <c r="O76" s="4">
+        <f t="shared" si="1"/>
+        <v>-6.3000000000000003E-4</v>
       </c>
     </row>
   </sheetData>
@@ -4395,13 +4730,13 @@
       <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="28.296875" customWidth="1"/>
-    <col min="8" max="8" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="20"/>
       <c r="B1" s="20"/>
       <c r="D1" s="20" t="s">
@@ -4409,7 +4744,7 @@
       </c>
       <c r="E1" s="20"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D2" s="14" t="s">
         <v>63</v>
       </c>
@@ -4417,7 +4752,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.399999999999999">
+    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D3" s="9" t="s">
         <v>100</v>
       </c>
@@ -4425,7 +4760,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.399999999999999">
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D4" s="9" t="s">
         <v>101</v>
       </c>
@@ -4433,7 +4768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.399999999999999">
+    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D5" s="9" t="s">
         <v>102</v>
       </c>
@@ -4441,7 +4776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.399999999999999">
+    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D6" s="9" t="s">
         <v>103</v>
       </c>
@@ -4449,7 +4784,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="17.399999999999999">
+    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D7" s="9" t="s">
         <v>104</v>
       </c>
@@ -4457,7 +4792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17.399999999999999">
+    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D8" s="9" t="s">
         <v>105</v>
       </c>
@@ -4465,7 +4800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17.399999999999999">
+    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D9" s="9" t="s">
         <v>106</v>
       </c>
@@ -4473,7 +4808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="17.399999999999999">
+    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D10" s="9" t="s">
         <v>107</v>
       </c>
@@ -4481,7 +4816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17.399999999999999">
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D11" s="9" t="s">
         <v>108</v>
       </c>
@@ -4489,7 +4824,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17.399999999999999">
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D12" s="9" t="s">
         <v>109</v>
       </c>
@@ -4497,7 +4832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17.399999999999999">
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D13" s="9" t="s">
         <v>110</v>
       </c>
@@ -4505,7 +4840,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17.399999999999999">
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D14" s="9" t="s">
         <v>111</v>
       </c>
@@ -4513,7 +4848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17.399999999999999">
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D15" s="9" t="s">
         <v>112</v>
       </c>
@@ -4521,7 +4856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17.399999999999999">
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D16" s="9" t="s">
         <v>89</v>
       </c>
@@ -4529,7 +4864,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="4:5" ht="17.399999999999999">
+    <row r="17" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D17" s="9" t="s">
         <v>116</v>
       </c>
@@ -4537,7 +4872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="4:5" ht="17.399999999999999">
+    <row r="18" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D18" s="9" t="s">
         <v>117</v>
       </c>
@@ -4545,7 +4880,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="4:5" ht="17.399999999999999">
+    <row r="19" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D19" s="9" t="s">
         <v>79</v>
       </c>
@@ -4553,7 +4888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="4:5" ht="17.399999999999999">
+    <row r="20" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D20" s="9" t="s">
         <v>118</v>
       </c>
@@ -4561,7 +4896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="4:5" ht="17.399999999999999">
+    <row r="21" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D21" s="9" t="s">
         <v>119</v>
       </c>
@@ -4569,7 +4904,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="4:5" ht="17.399999999999999">
+    <row r="22" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D22" s="9" t="s">
         <v>70</v>
       </c>
@@ -4577,7 +4912,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="4:5" ht="17.399999999999999">
+    <row r="23" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D23" s="9" t="s">
         <v>74</v>
       </c>
@@ -4585,7 +4920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="4:5" ht="17.399999999999999">
+    <row r="24" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D24" s="9" t="s">
         <v>120</v>
       </c>
@@ -4593,7 +4928,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="4:5" ht="17.399999999999999">
+    <row r="25" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D25" s="9" t="s">
         <v>121</v>
       </c>
@@ -4601,7 +4936,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="4:5" ht="17.399999999999999">
+    <row r="26" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D26" s="9" t="s">
         <v>122</v>
       </c>
@@ -4609,7 +4944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="4:5" ht="17.399999999999999">
+    <row r="27" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D27" s="9" t="s">
         <v>97</v>
       </c>
@@ -4617,7 +4952,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="4:5" ht="17.399999999999999">
+    <row r="28" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D28" s="9" t="s">
         <v>123</v>
       </c>
@@ -4625,7 +4960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="4:5" ht="17.399999999999999">
+    <row r="29" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D29" s="9" t="s">
         <v>83</v>
       </c>
@@ -4633,7 +4968,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="4:5" ht="17.399999999999999">
+    <row r="30" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D30" s="9" t="s">
         <v>86</v>
       </c>
@@ -4641,7 +4976,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="4:5" ht="17.399999999999999">
+    <row r="31" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D31" s="9" t="s">
         <v>124</v>
       </c>
@@ -4649,7 +4984,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="4:5" ht="17.399999999999999">
+    <row r="32" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D32" s="9" t="s">
         <v>88</v>
       </c>
@@ -4657,7 +4992,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="4:5" ht="17.399999999999999">
+    <row r="33" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D33" s="9" t="s">
         <v>125</v>
       </c>
@@ -4665,7 +5000,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="4:5" ht="17.399999999999999">
+    <row r="34" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D34" s="9" t="s">
         <v>87</v>
       </c>
@@ -4673,7 +5008,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="4:5" ht="17.399999999999999">
+    <row r="35" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D35" s="9" t="s">
         <v>126</v>
       </c>
@@ -4681,7 +5016,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="4:5" ht="17.399999999999999">
+    <row r="36" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D36" s="9" t="s">
         <v>82</v>
       </c>
@@ -4689,7 +5024,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="4:5" ht="17.399999999999999">
+    <row r="37" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D37" s="9" t="s">
         <v>127</v>
       </c>
@@ -4697,7 +5032,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="4:5" ht="17.399999999999999">
+    <row r="38" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D38" s="9" t="s">
         <v>129</v>
       </c>
@@ -4705,7 +5040,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="4:5" ht="17.399999999999999">
+    <row r="39" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D39" s="9" t="s">
         <v>130</v>
       </c>
@@ -4713,7 +5048,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="4:5" ht="17.399999999999999">
+    <row r="40" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D40" s="9" t="s">
         <v>131</v>
       </c>
@@ -4721,7 +5056,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="4:5" ht="17.399999999999999">
+    <row r="41" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D41" s="9" t="s">
         <v>132</v>
       </c>
@@ -4729,7 +5064,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="4:5" ht="17.399999999999999">
+    <row r="42" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D42" s="9" t="s">
         <v>133</v>
       </c>
@@ -4737,7 +5072,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="4:5" ht="17.399999999999999">
+    <row r="43" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D43" s="9" t="s">
         <v>134</v>
       </c>
@@ -4745,7 +5080,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="4:5" ht="17.399999999999999">
+    <row r="44" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D44" t="s">
         <v>135</v>
       </c>
@@ -4753,7 +5088,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="45" spans="4:5" ht="17.399999999999999">
+    <row r="45" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
         <v>136</v>
       </c>
@@ -4761,7 +5096,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="4:5" ht="17.399999999999999">
+    <row r="46" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D46" t="s">
         <v>137</v>
       </c>
@@ -4769,7 +5104,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="4:5" ht="17.399999999999999">
+    <row r="47" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
         <v>138</v>
       </c>
@@ -4777,7 +5112,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="4:5" ht="17.399999999999999">
+    <row r="48" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D48" s="12" t="s">
         <v>85</v>
       </c>
@@ -4785,7 +5120,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="4:9">
+    <row r="49" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D49" s="21" t="s">
         <v>144</v>
       </c>
@@ -4803,7 +5138,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="4:9" ht="17.399999999999999">
+    <row r="50" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D50" t="s">
         <v>68</v>
       </c>
@@ -4825,7 +5160,7 @@
         <v>1.2538591286300695</v>
       </c>
     </row>
-    <row r="51" spans="4:9" ht="17.399999999999999">
+    <row r="51" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D51" t="s">
         <v>73</v>
       </c>
@@ -4847,7 +5182,7 @@
         <v>0.24017792680380437</v>
       </c>
     </row>
-    <row r="52" spans="4:9" ht="17.399999999999999">
+    <row r="52" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D52" t="s">
         <v>75</v>
       </c>
@@ -4869,7 +5204,7 @@
         <v>0.12968709553009511</v>
       </c>
     </row>
-    <row r="53" spans="4:9" ht="17.399999999999999">
+    <row r="53" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D53" t="s">
         <v>76</v>
       </c>
@@ -4891,7 +5226,7 @@
         <v>0.15919071318394165</v>
       </c>
     </row>
-    <row r="54" spans="4:9" ht="17.399999999999999">
+    <row r="54" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D54" t="s">
         <v>78</v>
       </c>
@@ -4913,7 +5248,7 @@
         <v>3.8449204351271235E-2</v>
       </c>
     </row>
-    <row r="55" spans="4:9" ht="17.399999999999999">
+    <row r="55" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D55" t="s">
         <v>80</v>
       </c>
@@ -4935,7 +5270,7 @@
         <v>0.28142465287316215</v>
       </c>
     </row>
-    <row r="56" spans="4:9" ht="17.399999999999999">
+    <row r="56" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D56" t="s">
         <v>84</v>
       </c>
@@ -4957,7 +5292,7 @@
         <v>0.31620447007417013</v>
       </c>
     </row>
-    <row r="57" spans="4:9" ht="17.399999999999999">
+    <row r="57" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D57" t="s">
         <v>94</v>
       </c>
@@ -4979,7 +5314,7 @@
         <v>4.9496747283862979</v>
       </c>
     </row>
-    <row r="58" spans="4:9" ht="17.399999999999999">
+    <row r="58" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D58" t="s">
         <v>95</v>
       </c>
@@ -5001,7 +5336,7 @@
         <v>0.13208870841028206</v>
       </c>
     </row>
-    <row r="59" spans="4:9" ht="17.399999999999999">
+    <row r="59" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
         <v>96</v>
       </c>
@@ -5023,7 +5358,7 @@
         <v>0.19374627080710424</v>
       </c>
     </row>
-    <row r="60" spans="4:9" ht="17.399999999999999">
+    <row r="60" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D60" t="s">
         <v>98</v>
       </c>
@@ -5045,7 +5380,7 @@
         <v>0.73342003715408888</v>
       </c>
     </row>
-    <row r="61" spans="4:9" ht="17.399999999999999">
+    <row r="61" spans="4:9" ht="18" x14ac:dyDescent="0.2">
       <c r="D61" s="12" t="s">
         <v>99</v>
       </c>
@@ -5067,12 +5402,12 @@
         <v>0.21418461262022065</v>
       </c>
     </row>
-    <row r="62" spans="4:9">
+    <row r="62" spans="4:9" x14ac:dyDescent="0.2">
       <c r="D62" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="4:9" ht="34.799999999999997">
+    <row r="63" spans="4:9" ht="38" x14ac:dyDescent="0.2">
       <c r="D63" t="s">
         <v>149</v>
       </c>
@@ -5081,7 +5416,7 @@
       </c>
       <c r="F63" s="16"/>
     </row>
-    <row r="64" spans="4:9" ht="34.799999999999997">
+    <row r="64" spans="4:9" ht="38" x14ac:dyDescent="0.2">
       <c r="D64" s="12" t="s">
         <v>151</v>
       </c>
@@ -5090,14 +5425,14 @@
       </c>
       <c r="F64" s="16"/>
     </row>
-    <row r="65" spans="4:6" ht="17.399999999999999">
+    <row r="65" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D65" t="s">
         <v>172</v>
       </c>
       <c r="E65" s="17"/>
       <c r="F65" s="16"/>
     </row>
-    <row r="66" spans="4:6" ht="34.799999999999997">
+    <row r="66" spans="4:6" ht="38" x14ac:dyDescent="0.2">
       <c r="D66" s="12" t="s">
         <v>153</v>
       </c>
@@ -5106,14 +5441,14 @@
       </c>
       <c r="F66" s="16"/>
     </row>
-    <row r="67" spans="4:6" ht="17.399999999999999">
+    <row r="67" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D67" t="s">
         <v>173</v>
       </c>
       <c r="E67" s="17"/>
       <c r="F67" s="16"/>
     </row>
-    <row r="68" spans="4:6" ht="17.399999999999999">
+    <row r="68" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D68" t="s">
         <v>155</v>
       </c>
@@ -5122,7 +5457,7 @@
       </c>
       <c r="F68" s="16"/>
     </row>
-    <row r="69" spans="4:6" ht="17.399999999999999">
+    <row r="69" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D69" t="s">
         <v>157</v>
       </c>
@@ -5131,7 +5466,7 @@
       </c>
       <c r="F69" s="16"/>
     </row>
-    <row r="70" spans="4:6" ht="17.399999999999999">
+    <row r="70" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D70" t="s">
         <v>165</v>
       </c>
@@ -5140,7 +5475,7 @@
       </c>
       <c r="F70" s="16"/>
     </row>
-    <row r="71" spans="4:6" ht="17.399999999999999">
+    <row r="71" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D71" t="s">
         <v>168</v>
       </c>
@@ -5149,18 +5484,18 @@
       </c>
       <c r="F71" s="16"/>
     </row>
-    <row r="72" spans="4:6" ht="17.399999999999999">
+    <row r="72" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="E72" s="17"/>
       <c r="F72" s="16"/>
     </row>
-    <row r="73" spans="4:6" ht="17.399999999999999">
+    <row r="73" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D73" s="12" t="s">
         <v>140</v>
       </c>
       <c r="E73" s="18"/>
       <c r="F73" s="16"/>
     </row>
-    <row r="74" spans="4:6" ht="17.399999999999999">
+    <row r="74" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D74" s="11" t="s">
         <v>113</v>
       </c>
@@ -5168,7 +5503,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="4:6" ht="17.399999999999999">
+    <row r="75" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D75" s="11" t="s">
         <v>114</v>
       </c>
@@ -5176,7 +5511,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="4:6" ht="17.399999999999999">
+    <row r="76" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D76" s="11" t="s">
         <v>115</v>
       </c>
@@ -5184,7 +5519,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="77" spans="4:6" ht="17.399999999999999">
+    <row r="77" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D77" t="s">
         <v>139</v>
       </c>
@@ -5192,7 +5527,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="78" spans="4:6" ht="17.399999999999999">
+    <row r="78" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D78" t="s">
         <v>66</v>
       </c>
@@ -5200,7 +5535,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="79" spans="4:6" ht="17.399999999999999">
+    <row r="79" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D79" t="s">
         <v>67</v>
       </c>
@@ -5208,7 +5543,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="80" spans="4:6" ht="17.399999999999999">
+    <row r="80" spans="4:6" ht="18" x14ac:dyDescent="0.2">
       <c r="D80" t="s">
         <v>69</v>
       </c>
@@ -5216,7 +5551,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="81" spans="4:5" ht="17.399999999999999">
+    <row r="81" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D81" t="s">
         <v>71</v>
       </c>
@@ -5224,7 +5559,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="82" spans="4:5" ht="17.399999999999999">
+    <row r="82" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D82" t="s">
         <v>72</v>
       </c>
@@ -5232,7 +5567,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="83" spans="4:5" ht="17.399999999999999">
+    <row r="83" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D83" t="s">
         <v>77</v>
       </c>
@@ -5240,7 +5575,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="84" spans="4:5" ht="17.399999999999999">
+    <row r="84" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D84" t="s">
         <v>81</v>
       </c>
@@ -5248,7 +5583,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="85" spans="4:5" ht="17.399999999999999">
+    <row r="85" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D85" t="s">
         <v>90</v>
       </c>
@@ -5256,7 +5591,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="86" spans="4:5" ht="17.399999999999999">
+    <row r="86" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D86" t="s">
         <v>91</v>
       </c>
@@ -5264,7 +5599,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="87" spans="4:5" ht="17.399999999999999">
+    <row r="87" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D87" t="s">
         <v>92</v>
       </c>
@@ -5272,7 +5607,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="88" spans="4:5" ht="17.399999999999999">
+    <row r="88" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D88" t="s">
         <v>93</v>
       </c>
@@ -5280,7 +5615,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="89" spans="4:5" ht="17.399999999999999">
+    <row r="89" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D89" t="s">
         <v>159</v>
       </c>
@@ -5288,7 +5623,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="90" spans="4:5" ht="17.399999999999999">
+    <row r="90" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D90" t="s">
         <v>160</v>
       </c>
@@ -5296,7 +5631,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="91" spans="4:5" ht="17.399999999999999">
+    <row r="91" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D91" t="s">
         <v>161</v>
       </c>
@@ -5304,7 +5639,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="92" spans="4:5" ht="17.399999999999999">
+    <row r="92" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D92" t="s">
         <v>162</v>
       </c>
@@ -5312,7 +5647,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="93" spans="4:5" ht="17.399999999999999">
+    <row r="93" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D93" t="s">
         <v>163</v>
       </c>
@@ -5320,7 +5655,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="94" spans="4:5" ht="17.399999999999999">
+    <row r="94" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D94" t="s">
         <v>164</v>
       </c>
@@ -5328,13 +5663,13 @@
         <v>140</v>
       </c>
     </row>
-    <row r="96" spans="4:5">
+    <row r="96" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D96" s="12" t="s">
         <v>170</v>
       </c>
       <c r="E96" s="12"/>
     </row>
-    <row r="97" spans="4:5" ht="17.399999999999999">
+    <row r="97" spans="4:5" ht="18" x14ac:dyDescent="0.2">
       <c r="D97" s="19" t="s">
         <v>128</v>
       </c>

</xml_diff>